<commit_message>
Mise à jour planning et nbr de pages à faire
</commit_message>
<xml_diff>
--- a/drafts/Planning.xlsx
+++ b/drafts/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33616\Desktop\MemoireDeRechercheMaster2\drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE396754-09C0-42E2-B03E-C9EF498FEE62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42FC76F-2557-48B3-9EA0-8583A99D3EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{740A0355-2552-4D02-AF72-2E561246BC34}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>ORAL</t>
   </si>
@@ -57,9 +56,6 @@
     <t>JUILLET</t>
   </si>
   <si>
-    <t>Entretiens finis</t>
-  </si>
-  <si>
     <t>REDACTION</t>
   </si>
   <si>
@@ -130,13 +126,34 @@
   </si>
   <si>
     <t>Présentation 1/3</t>
+  </si>
+  <si>
+    <t>RENDU</t>
+  </si>
+  <si>
+    <t>16/3 : Revue complète</t>
+  </si>
+  <si>
+    <t>20/4 : Plan de collecte complète</t>
+  </si>
+  <si>
+    <t>23/2 : Intro + Revue v1</t>
+  </si>
+  <si>
+    <t>Entretiens finis + 1/3 rédigé</t>
+  </si>
+  <si>
+    <t>20/5 : mémoire à 75%</t>
+  </si>
+  <si>
+    <t>20/6 : mémoire à 100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +229,21 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Iskoola Pota"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
       <name val="Iskoola Pota"/>
       <family val="2"/>
     </font>
@@ -256,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -486,6 +518,56 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -496,7 +578,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -561,9 +643,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -574,6 +653,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="3" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C020900D-6B45-49B0-8788-5CD37467A421}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
@@ -906,8 +1003,8 @@
     <col min="2" max="2" width="23.47265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5234375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.62890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.89453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.3125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.9453125" style="1"/>
   </cols>
@@ -935,135 +1032,158 @@
     </row>
     <row r="2" spans="1:7" ht="15.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="20" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="11"/>
       <c r="D6" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="21" t="s">
+      <c r="A7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="B7" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="31">
+        <v>44022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="F8" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.6" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="9" spans="1:7" ht="15.6" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="24" t="s">
-        <v>22</v>
+      <c r="B12" s="22" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="25" t="s">
-        <v>26</v>
+      <c r="B13" s="23" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="26" t="s">
-        <v>27</v>
+      <c r="B14" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revue de littérature - BQR
Brand Quality Relationship - Helme-Guizon & Magnoni - brouillon d'une première analyse du texte
</commit_message>
<xml_diff>
--- a/drafts/Planning.xlsx
+++ b/drafts/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33616\Desktop\MemoireDeRechercheMaster2\drafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42FC76F-2557-48B3-9EA0-8583A99D3EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91513BD-6AF6-4DFF-8096-F8D966B79694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{740A0355-2552-4D02-AF72-2E561246BC34}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>ORAL</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Ccls - 3 pages</t>
   </si>
   <si>
-    <t>Finies</t>
-  </si>
-  <si>
     <t>Relecture et correction</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>Validé</t>
   </si>
   <si>
-    <t>Rédaction finie</t>
-  </si>
-  <si>
     <t>1/4 rédigée</t>
   </si>
   <si>
@@ -131,22 +125,31 @@
     <t>RENDU</t>
   </si>
   <si>
-    <t>16/3 : Revue complète</t>
-  </si>
-  <si>
     <t>20/4 : Plan de collecte complète</t>
   </si>
   <si>
     <t>23/2 : Intro + Revue v1</t>
   </si>
   <si>
-    <t>Entretiens finis + 1/3 rédigé</t>
-  </si>
-  <si>
     <t>20/5 : mémoire à 75%</t>
   </si>
   <si>
     <t>20/6 : mémoire à 100%</t>
+  </si>
+  <si>
+    <t>Rédaction finie - 20 pages</t>
+  </si>
+  <si>
+    <t>Rédaction finie - 10 pages</t>
+  </si>
+  <si>
+    <t>1/4 rédigé</t>
+  </si>
+  <si>
+    <t>Entretiens finis + 1/2 rédigé</t>
+  </si>
+  <si>
+    <t>15/3 : Revue complète</t>
   </si>
 </sst>
 </file>
@@ -994,16 +997,16 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="29.9453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.62890625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.62890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.89453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.62890625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.3125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.9453125" style="1"/>
@@ -1038,16 +1041,16 @@
         <v>13</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="13"/>
     </row>
@@ -1056,17 +1059,17 @@
         <v>8</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>20</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="14"/>
     </row>
@@ -1075,15 +1078,15 @@
         <v>9</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="14"/>
     </row>
@@ -1092,19 +1095,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="14"/>
     </row>
@@ -1115,34 +1118,34 @@
       <c r="B6" s="9"/>
       <c r="C6" s="11"/>
       <c r="D6" s="18" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E6" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>16</v>
       </c>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>34</v>
-      </c>
       <c r="C7" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="F7" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="G7" s="31">
         <v>44022</v>
@@ -1156,10 +1159,10 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>0</v>
@@ -1168,22 +1171,22 @@
     <row r="9" spans="1:7" ht="15.6" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>